<commit_message>
adding to close and reopen browser between methods
</commit_message>
<xml_diff>
--- a/src/test/java/testData/HFHS_Keywords.xlsx
+++ b/src/test/java/testData/HFHS_Keywords.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Keyword</t>
   </si>
@@ -45,6 +45,24 @@
   </si>
   <si>
     <t>His First His Second</t>
+  </si>
+  <si>
+    <t>B00XNZ0IZQ</t>
+  </si>
+  <si>
+    <t>The Dead and the Missing</t>
+  </si>
+  <si>
+    <t>Thrillers</t>
+  </si>
+  <si>
+    <t>Private Detective</t>
+  </si>
+  <si>
+    <t>Private Detective Series</t>
+  </si>
+  <si>
+    <t>Crime Fiction</t>
   </si>
 </sst>
 </file>
@@ -362,13 +380,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -403,6 +425,50 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed for longer runs
</commit_message>
<xml_diff>
--- a/src/test/java/testData/HFHS_Keywords.xlsx
+++ b/src/test/java/testData/HFHS_Keywords.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Keyword</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>Crime Fiction</t>
+  </si>
+  <si>
+    <t>B01531YHYU</t>
+  </si>
+  <si>
+    <t>Project Return Fire</t>
+  </si>
+  <si>
+    <t>Action Adventure</t>
+  </si>
+  <si>
+    <t>Time Travel Action Adventure</t>
+  </si>
+  <si>
+    <t>Science Fiction Action Adventure</t>
+  </si>
+  <si>
+    <t>Science Fiction</t>
   </si>
 </sst>
 </file>
@@ -380,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +487,50 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>